<commit_message>
Completed basic line xlsx
</commit_message>
<xml_diff>
--- a/file_parsing_service/xlsx/basic_line.xlsx
+++ b/file_parsing_service/xlsx/basic_line.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/george/Repos/javascript/SaaS23-08/file_parsing_service/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C48524E-038F-0145-9685-B0E18ABF238D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D4E736-AFDF-2C44-B6A5-153B6D959898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3200" yWindow="14900" windowWidth="28800" windowHeight="17500" xr2:uid="{FED25B8F-62BB-0943-9034-926BEC444857}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
   <si>
     <t>This is the series 1 name</t>
   </si>
@@ -52,12 +52,6 @@
     <t># leave empty if you don't want one</t>
   </si>
   <si>
-    <t># number, the first x-axis point</t>
-  </si>
-  <si>
-    <t># number, the difference between two consecutive x-axis points</t>
-  </si>
-  <si>
     <t># x values</t>
   </si>
   <si>
@@ -85,12 +79,6 @@
     <t>series/1/marker/enabled</t>
   </si>
   <si>
-    <t>series/1/pointStart</t>
-  </si>
-  <si>
-    <t>series/1/pointInterval</t>
-  </si>
-  <si>
     <t>series/1/data/x</t>
   </si>
   <si>
@@ -112,26 +100,180 @@
     <t>series/2/marker/enabled</t>
   </si>
   <si>
-    <t>series/2/pointStart</t>
-  </si>
-  <si>
-    <t>series/2/pointInterval</t>
-  </si>
-  <si>
     <t>series/2/data/x</t>
   </si>
   <si>
     <t>series/2/data/y</t>
+  </si>
+  <si>
+    <t># ----------------------------------------</t>
+  </si>
+  <si>
+    <t># Options regarding the title of the chart</t>
+  </si>
+  <si>
+    <t>title/text</t>
+  </si>
+  <si>
+    <t>This is the title\, which contains a comma</t>
+  </si>
+  <si>
+    <t># left, center, right (ignored if title text is empty)</t>
+  </si>
+  <si>
+    <t>title/align</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t># top, middle, bottom (ignored if title text is empty)</t>
+  </si>
+  <si>
+    <t>title/verticalAlign</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t># -------------------------------------------</t>
+  </si>
+  <si>
+    <t># Options regarding the subtitle of the chart</t>
+  </si>
+  <si>
+    <t>subtitle/text</t>
+  </si>
+  <si>
+    <t>This is the subtitle</t>
+  </si>
+  <si>
+    <t># left, center, right (ignored if subtitle text is empty)</t>
+  </si>
+  <si>
+    <t>subtitle/align</t>
+  </si>
+  <si>
+    <t># top, middle, bottom (ignored if subtitle text is empty)</t>
+  </si>
+  <si>
+    <t>subtitle/verticalAlign</t>
+  </si>
+  <si>
+    <t># ------------------------------------------</t>
+  </si>
+  <si>
+    <t># Options regarding the caption of the chart</t>
+  </si>
+  <si>
+    <t>caption/text</t>
+  </si>
+  <si>
+    <t>This is the caption</t>
+  </si>
+  <si>
+    <t># left, center, right (ignored if caption text is empty)</t>
+  </si>
+  <si>
+    <t>caption/align</t>
+  </si>
+  <si>
+    <t># top, middle, bottom (ignored if caption text is empty)</t>
+  </si>
+  <si>
+    <t>caption/verticalAlign</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t># Options regarding the legend of the chart</t>
+  </si>
+  <si>
+    <t># true, false</t>
+  </si>
+  <si>
+    <t>legend/enabled</t>
+  </si>
+  <si>
+    <t># left, center, right (ignored if legend is disabled)</t>
+  </si>
+  <si>
+    <t>legend/align</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t># top, middle, bottom (ignored if legend is disabled)</t>
+  </si>
+  <si>
+    <t>legend/verticalAlign</t>
+  </si>
+  <si>
+    <t># -----------------------------------------------------------</t>
+  </si>
+  <si>
+    <t># Options regarding the x-axis (horizontal axis) of the chart</t>
+  </si>
+  <si>
+    <t>xAxis/title/text</t>
+  </si>
+  <si>
+    <t>This is the x-axis title</t>
+  </si>
+  <si>
+    <t># linear, logarithmic, category</t>
+  </si>
+  <si>
+    <t>xAxis/type</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t># ---------------------------------------------------------</t>
+  </si>
+  <si>
+    <t># Options regarding the y-axis (vertical axis) of the chart</t>
+  </si>
+  <si>
+    <t>yAxis/title/text</t>
+  </si>
+  <si>
+    <t>This is the y-axis title</t>
+  </si>
+  <si>
+    <t>yAxis/type</t>
+  </si>
+  <si>
+    <t># ---------------------------------------</t>
+  </si>
+  <si>
+    <t># Set to true if you want to swap the two axes</t>
+  </si>
+  <si>
+    <t># &lt;true, false&gt;</t>
+  </si>
+  <si>
+    <t>chart/inverted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,9 +299,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -476,16 +621,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF355A02-5E87-EA47-BD20-8FAC40F3EFF3}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N53" sqref="N53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="86.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="1"/>
@@ -508,17 +653,17 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -528,315 +673,589 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="1">
-        <v>-5</v>
-      </c>
-      <c r="C27" s="1">
-        <v>-4</v>
-      </c>
-      <c r="D27" s="1">
-        <v>-3</v>
-      </c>
-      <c r="E27" s="1">
-        <v>-2</v>
-      </c>
-      <c r="F27" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G27" s="1">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1">
-        <v>1</v>
-      </c>
-      <c r="I27" s="1">
-        <v>2</v>
-      </c>
-      <c r="J27" s="1">
-        <v>3</v>
-      </c>
-      <c r="K27" s="1">
-        <v>4</v>
-      </c>
-      <c r="L27" s="1">
-        <v>5</v>
-      </c>
-      <c r="M27" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="1">
-        <v>10</v>
-      </c>
-      <c r="C30" s="1">
-        <v>15</v>
-      </c>
-      <c r="D30" s="1">
-        <v>14</v>
-      </c>
-      <c r="E30" s="1">
-        <v>17</v>
-      </c>
-      <c r="F30" s="1">
-        <v>46</v>
-      </c>
-      <c r="G30" s="1">
-        <v>55</v>
-      </c>
-      <c r="H30" s="1">
-        <v>34</v>
-      </c>
-      <c r="I30" s="1">
-        <v>22</v>
-      </c>
-      <c r="J30" s="1">
-        <v>5</v>
-      </c>
-      <c r="K30" s="1">
-        <v>-3</v>
-      </c>
-      <c r="L30" s="1">
-        <v>-9</v>
-      </c>
-      <c r="M30" s="1">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="1">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>6</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50" s="1">
-        <v>-10</v>
-      </c>
-      <c r="C50" s="1">
-        <v>-9</v>
-      </c>
-      <c r="D50" s="1">
-        <v>-7</v>
-      </c>
-      <c r="E50" s="1">
-        <v>-6</v>
-      </c>
-      <c r="F50" s="1">
-        <v>-5</v>
-      </c>
-      <c r="G50" s="1">
-        <v>-3</v>
-      </c>
-      <c r="H50" s="1">
-        <v>0</v>
-      </c>
-      <c r="I50" s="1">
-        <v>2</v>
-      </c>
-      <c r="J50" s="1">
-        <v>3</v>
-      </c>
-      <c r="K50" s="1">
-        <v>4</v>
-      </c>
-      <c r="L50" s="1">
-        <v>6</v>
-      </c>
-      <c r="M50" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B53" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B96" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B114" s="1">
+        <v>-5</v>
+      </c>
+      <c r="C114" s="1">
+        <v>-4</v>
+      </c>
+      <c r="D114" s="1">
+        <v>-3</v>
+      </c>
+      <c r="E114" s="1">
+        <v>-2</v>
+      </c>
+      <c r="F114" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G114" s="1">
+        <v>0</v>
+      </c>
+      <c r="H114" s="1">
+        <v>1</v>
+      </c>
+      <c r="I114" s="1">
         <v>2</v>
       </c>
-      <c r="C53" s="1">
+      <c r="J114" s="1">
         <v>3</v>
       </c>
-      <c r="D53" s="1">
+      <c r="K114" s="1">
         <v>4</v>
       </c>
-      <c r="E53" s="1">
+      <c r="L114" s="1">
         <v>5</v>
       </c>
-      <c r="F53" s="1">
+      <c r="M114" s="1">
         <v>6</v>
       </c>
-      <c r="G53" s="1">
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B117" s="1">
+        <v>10</v>
+      </c>
+      <c r="C117" s="1">
+        <v>15</v>
+      </c>
+      <c r="D117" s="1">
+        <v>14</v>
+      </c>
+      <c r="E117" s="1">
+        <v>17</v>
+      </c>
+      <c r="F117" s="1">
+        <v>46</v>
+      </c>
+      <c r="G117" s="1">
+        <v>55</v>
+      </c>
+      <c r="H117" s="1">
+        <v>34</v>
+      </c>
+      <c r="I117" s="1">
+        <v>22</v>
+      </c>
+      <c r="J117" s="1">
+        <v>5</v>
+      </c>
+      <c r="K117" s="1">
+        <v>-3</v>
+      </c>
+      <c r="L117" s="1">
+        <v>-9</v>
+      </c>
+      <c r="M117" s="1">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B125" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B128" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B131" s="1">
+        <v>-10</v>
+      </c>
+      <c r="C131" s="1">
+        <v>-9</v>
+      </c>
+      <c r="D131" s="1">
+        <v>-7</v>
+      </c>
+      <c r="E131" s="1">
+        <v>-6</v>
+      </c>
+      <c r="F131" s="1">
+        <v>-5</v>
+      </c>
+      <c r="G131" s="1">
+        <v>-3</v>
+      </c>
+      <c r="H131" s="1">
+        <v>0</v>
+      </c>
+      <c r="I131" s="1">
+        <v>2</v>
+      </c>
+      <c r="J131" s="1">
+        <v>3</v>
+      </c>
+      <c r="K131" s="1">
+        <v>4</v>
+      </c>
+      <c r="L131" s="1">
+        <v>6</v>
+      </c>
+      <c r="M131" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B134" s="1">
+        <v>2</v>
+      </c>
+      <c r="C134" s="1">
+        <v>3</v>
+      </c>
+      <c r="D134" s="1">
+        <v>4</v>
+      </c>
+      <c r="E134" s="1">
+        <v>5</v>
+      </c>
+      <c r="F134" s="1">
+        <v>6</v>
+      </c>
+      <c r="G134" s="1">
         <v>7</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H134" s="1">
         <v>8</v>
       </c>
-      <c r="I53" s="1">
+      <c r="I134" s="1">
         <v>9</v>
       </c>
-      <c r="J53" s="1">
+      <c r="J134" s="1">
         <v>10</v>
       </c>
-      <c r="K53" s="1">
+      <c r="K134" s="1">
         <v>12</v>
       </c>
-      <c r="L53" s="1">
+      <c r="L134" s="1">
         <v>13</v>
       </c>
-      <c r="M53" s="1">
+      <c r="M134" s="1">
         <v>15</v>
       </c>
     </row>

</xml_diff>